<commit_message>
Added EfficientDet D1 results.
</commit_message>
<xml_diff>
--- a/report_raw.xlsx
+++ b/report_raw.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>model</t>
+          <t>Model</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -530,212 +530,212 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>efficientdet_d0_coco17_tpu-32</t>
+          <t>centernet_resnet50_v2_512x512_coco17_tpu-8_bsize_16</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.08021096856360015</v>
+        <v>0.9909523809523809</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08021096856360015</v>
+        <v>0.990952380952381</v>
       </c>
       <c r="D5" t="n">
-        <v>0.096</v>
+        <v>0.988</v>
       </c>
       <c r="E5" t="n">
-        <v>0.09600000000000002</v>
+        <v>0.9880000000000001</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4663673943304381</v>
+        <v>0.9693082883029307</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>efficientdet_d0_coco17_tpu-32_bsize_16</t>
+          <t>efficientdet_d0_coco17_tpu-32</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9842857142857143</v>
+        <v>0.08021096856360015</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9842857142857143</v>
+        <v>0.08021096856360015</v>
       </c>
       <c r="D6" t="n">
-        <v>0.98</v>
+        <v>0.096</v>
       </c>
       <c r="E6" t="n">
-        <v>0.98</v>
+        <v>0.09600000000000002</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9589378331860516</v>
+        <v>0.4663673943304381</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>faster_rcnn_resnet152_v1_640x640_coco17_tpu-8</t>
+          <t>efficientdet_d0_coco17_tpu-32_bsize_16</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0012814219212865</v>
+        <v>0.9842857142857143</v>
       </c>
       <c r="C7" t="n">
-        <v>0.001256296001261275</v>
+        <v>0.9842857142857143</v>
       </c>
       <c r="D7" t="n">
-        <v>0.028</v>
+        <v>0.98</v>
       </c>
       <c r="E7" t="n">
-        <v>0.02745098039215686</v>
+        <v>0.98</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6721566085354743</v>
+        <v>0.9589378331860516</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>faster_rcnn_resnet50_v1_640x640_coco17_tpu-8</t>
+          <t>efficientdet_d1_coco17_tpu-32</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.005380844645550528</v>
+        <v>0.0299010899010899</v>
       </c>
       <c r="C8" t="n">
-        <v>0.005275337887794635</v>
+        <v>0.02931479402067638</v>
       </c>
       <c r="D8" t="n">
-        <v>0.044</v>
+        <v>0.04</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04313725490196079</v>
+        <v>0.0392156862745098</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8696119053152483</v>
+        <v>0.4228139897782832</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>faster_rcnn_resnet50_v1_640x640_coco17_tpu-8_bsize_8</t>
+          <t>efficientdet_d1_coco17_tpu-32_bsize_8</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9062301587301588</v>
+        <v>0.9933333333333334</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9062301587301588</v>
+        <v>0.9933333333333334</v>
       </c>
       <c r="D9" t="n">
-        <v>0.88</v>
+        <v>0.992</v>
       </c>
       <c r="E9" t="n">
-        <v>0.88</v>
+        <v>0.9919999999999999</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9604807039437974</v>
+        <v>0.9641992746040781</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>ssd_resnet101_v1_fpn_640x640_coco17_tpu-8</t>
+          <t>faster_rcnn_resnet152_v1_640x640_coco17_tpu-8</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.001212121212121212</v>
+        <v>0.0012814219212865</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0011883541295306</v>
+        <v>0.001256296001261275</v>
       </c>
       <c r="D10" t="n">
-        <v>0.016</v>
+        <v>0.028</v>
       </c>
       <c r="E10" t="n">
-        <v>0.01568627450980392</v>
+        <v>0.02745098039215686</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8649898653394632</v>
+        <v>0.6721566085354743</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>ssd_resnet101_v1_fpn_640x640_coco17_tpu-8_bsize_16</t>
+          <t>faster_rcnn_resnet152_v1_640x640_coco17_tpu-8_bsize_8</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.6810625485625486</v>
+        <v>0.9626190476190477</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6810625485625486</v>
+        <v>0.9626190476190476</v>
       </c>
       <c r="D11" t="n">
-        <v>0.64</v>
+        <v>0.948</v>
       </c>
       <c r="E11" t="n">
-        <v>0.64</v>
+        <v>0.9479999999999998</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9082607077268948</v>
+        <v>0.9736932490821781</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>ssd_resnet152_v1_fpn_640x640_coco17_tpu-8</t>
+          <t>faster_rcnn_resnet50_v1_640x640_coco17_tpu-8</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.01625162531856244</v>
+        <v>0.005380844645550528</v>
       </c>
       <c r="C12" t="n">
-        <v>0.01593296599859063</v>
+        <v>0.005275337887794635</v>
       </c>
       <c r="D12" t="n">
-        <v>0.052</v>
+        <v>0.044</v>
       </c>
       <c r="E12" t="n">
-        <v>0.05098039215686274</v>
+        <v>0.04313725490196079</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7729092831740644</v>
+        <v>0.8696119053152483</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>ssd_resnet152_v1_fpn_640x640_coco17_tpu-8_bsize_16</t>
+          <t>faster_rcnn_resnet50_v1_640x640_coco17_tpu-8_bsize_8</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.7209603174603175</v>
+        <v>0.9062301587301588</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7209603174603174</v>
+        <v>0.9062301587301588</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6840000000000001</v>
+        <v>0.88</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6840000000000001</v>
+        <v>0.88</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9744815513795926</v>
+        <v>0.9604807039437974</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>ssd_resnet50_v1_fpn_640x640_coco17_tpu-8</t>
+          <t>ssd_resnet101_v1_fpn_640x640_coco17_tpu-8</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0008080808080808082</v>
+        <v>0.001212121212121212</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0007922360863537335</v>
+        <v>0.0011883541295306</v>
       </c>
       <c r="D14" t="n">
         <v>0.016</v>
@@ -744,138 +744,248 @@
         <v>0.01568627450980392</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1708097251213045</v>
+        <v>0.8649898653394632</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>ssd_resnet50_v1_fpn_640x640_coco17_tpu-8_bsize_16</t>
+          <t>ssd_resnet101_v1_fpn_640x640_coco17_tpu-8_bsize_16</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.5217443184834488</v>
+        <v>0.6810625485625486</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5217443184834489</v>
+        <v>0.6810625485625486</v>
       </c>
       <c r="D15" t="n">
-        <v>0.452</v>
+        <v>0.64</v>
       </c>
       <c r="E15" t="n">
-        <v>0.452</v>
+        <v>0.64</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9361229425352515</v>
+        <v>0.9082607077268948</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>yolov8m_lego_416_bsize_16</t>
+          <t>ssd_resnet152_v1_fpn_640x640_coco17_tpu-8</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9966666666666667</v>
+        <v>0.01625162531856244</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9966666666666667</v>
+        <v>0.01593296599859063</v>
       </c>
       <c r="D16" t="n">
-        <v>0.996</v>
+        <v>0.052</v>
       </c>
       <c r="E16" t="n">
-        <v>0.996</v>
+        <v>0.05098039215686274</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9620959358531538</v>
+        <v>0.7729092831740644</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>yolov8n_lego_416_bsize_1</t>
+          <t>ssd_resnet152_v1_fpn_640x640_coco17_tpu-8_bsize_16</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.4310121312379376</v>
+        <v>0.7209603174603175</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4225609129783702</v>
+        <v>0.7209603174603174</v>
       </c>
       <c r="D17" t="n">
-        <v>0.424</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="E17" t="n">
-        <v>0.415686274509804</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="F17" t="n">
-        <v>0.8491738095221806</v>
+        <v>0.9744815513795926</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>yolov8n_lego_416_bsize_16</t>
+          <t>ssd_resnet50_v1_fpn_640x640_coco17_tpu-8</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.9786666666666668</v>
+        <v>0.0008080808080808082</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9786666666666668</v>
+        <v>0.0007922360863537335</v>
       </c>
       <c r="D18" t="n">
-        <v>0.976</v>
+        <v>0.016</v>
       </c>
       <c r="E18" t="n">
-        <v>0.976</v>
+        <v>0.01568627450980392</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9612300542185918</v>
+        <v>0.1708097251213045</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>yolov8n_lego_416_bsize_32</t>
+          <t>ssd_resnet50_v1_fpn_640x640_coco17_tpu-8_bsize_16</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.9853333333333334</v>
+        <v>0.5217443184834488</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9853333333333333</v>
+        <v>0.5217443184834489</v>
       </c>
       <c r="D19" t="n">
-        <v>0.984</v>
+        <v>0.452</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9840000000000001</v>
+        <v>0.452</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9611797106409827</v>
+        <v>0.9361229425352515</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
+          <t>yolov8m_lego_416_bsize_16</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.9966666666666667</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9966666666666667</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9620959358531538</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>yolov8m_lego_416_bsize_8</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.9933333333333334</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.9933333333333334</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.992</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.992</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.9610137022932269</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>yolov8n_lego_416_bsize_1</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.4310121312379376</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.4225609129783702</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.424</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.415686274509804</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.8491738095221806</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>yolov8n_lego_416_bsize_16</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.9786666666666668</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.9786666666666668</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.976</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.976</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.9612300542185918</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>yolov8n_lego_416_bsize_32</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.9853333333333334</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.9853333333333333</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.984</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.9840000000000001</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.9611797106409827</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
           <t>yolov8n_lego_416_bsize_8</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B25" t="n">
         <v>0.9886666666666667</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C25" t="n">
         <v>0.9886666666666667</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D25" t="n">
         <v>0.988</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E25" t="n">
         <v>0.9880000000000001</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F25" t="n">
         <v>0.9608917226838777</v>
       </c>
     </row>

</xml_diff>